<commit_message>
Updated Gaant Chart, Updated Project Plan and Updated Software Design Document
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf6ef4105294d07f/Documents/Software Technologies Assigment/2810ICT-7810ICT-Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchav\Documents\AA Uni\2810ICT - Software Technologies\Assignments\A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="233" documentId="11_E0C8A7F0515C29AAE5B1393562E56DCE2A14542E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{036E437B-80F6-4605-8DBC-483B3BB8C885}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026C6CC9-98BC-41F2-82D7-5A3DC991A8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -639,12 +639,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -665,18 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -845,10 +845,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1084,24 +1080,24 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BT9" activeCellId="1" sqref="DD12 BT9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
-    <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="2.75" style="1"/>
+    <col min="42" max="42" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
         <v>42</v>
       </c>
@@ -1111,14 +1107,14 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1126,37 +1122,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="29"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="31" t="s">
+      <c r="V2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="33"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="31" t="s">
+      <c r="AA2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="33"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
         <v>14</v>
@@ -1169,23 +1165,23 @@
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="30" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1211,13 +1207,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1399,7 +1395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
@@ -1419,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:67" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>33</v>
       </c>
@@ -1439,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:67" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1459,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:67" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>35</v>
       </c>
@@ -1479,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:67" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="24" t="s">
         <v>36</v>
       </c>
@@ -1499,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:67" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>37</v>
       </c>
@@ -1519,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:67" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
@@ -1536,10 +1532,10 @@
         <v>16</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="73.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
@@ -1556,10 +1552,10 @@
         <v>18</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
         <v>40</v>
       </c>
@@ -1576,10 +1572,10 @@
         <v>21</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
@@ -1596,10 +1592,10 @@
         <v>24</v>
       </c>
       <c r="G14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>48</v>
       </c>
@@ -1616,10 +1612,10 @@
         <v>24</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="60.6" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>43</v>
       </c>
@@ -1636,10 +1632,10 @@
         <v>24</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>44</v>
       </c>
@@ -1655,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>45</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>46</v>
       </c>
@@ -1687,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>49</v>
       </c>
@@ -1703,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>2</v>
       </c>
@@ -1715,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>3</v>
       </c>
@@ -1727,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1739,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>5</v>
       </c>
@@ -1751,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>6</v>
       </c>
@@ -1763,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>7</v>
       </c>
@@ -1775,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>8</v>
       </c>
@@ -1787,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>9</v>
       </c>
@@ -1799,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>10</v>
       </c>
@@ -1811,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
         <v>11</v>
       </c>
@@ -1823,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>23</v>
       </c>
@@ -1835,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
         <v>24</v>
       </c>
@@ -1847,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
         <v>25</v>
       </c>
@@ -1859,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
         <v>26</v>
       </c>
@@ -1871,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
         <v>27</v>
       </c>
@@ -1883,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
         <v>28</v>
       </c>
@@ -1895,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6" t="s">
         <v>29</v>
       </c>
@@ -1907,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
         <v>30</v>
       </c>
@@ -1919,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
         <v>31</v>
       </c>
@@ -1933,17 +1929,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">
@@ -2008,4 +2004,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c9f92db8-2851-4df9-9d12-fab52f5b1415}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
executive summary and updates
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchav\Documents\AA Uni\2810ICT - Software Technologies\Assignments\A1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf6ef4105294d07f/Documents/GitHub/2810ICT-7810ICT-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026C6CC9-98BC-41F2-82D7-5A3DC991A8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{026C6CC9-98BC-41F2-82D7-5A3DC991A8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA2F027C-2196-49C3-8CF7-69C2BF6CC7F3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -56,27 +56,6 @@
     <t>ACTIVITY</t>
   </si>
   <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
     <t>Activity 24</t>
   </si>
   <si>
@@ -254,22 +233,43 @@
     <t>#012 Downloading git_log.txt</t>
   </si>
   <si>
-    <t>#013 Code for Data Analysis</t>
-  </si>
-  <si>
-    <t>#014 Preparing the User Manual.docx</t>
-  </si>
-  <si>
-    <t>#015 Creating Software Testing Report.docx</t>
-  </si>
-  <si>
     <t xml:space="preserve">PLAN START </t>
   </si>
   <si>
     <t xml:space="preserve">#011 Including the Gantt Chart in the Project Plan Document </t>
   </si>
   <si>
-    <t>#016 Preparing the Executive Summary.docx</t>
+    <t xml:space="preserve">#013     Writing the code for Feature 1 </t>
+  </si>
+  <si>
+    <t>#014     Writing the code for Feature 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#015     Writing the code for Feature 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#016     Writing the code for Feature 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#017     Writing the code for Feature 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#018     Creating a Software Testing Report.docx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#019     Preparing the Executive Summary.docx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#020     Updating Project Plan.docx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#021     Updating Software Design Document.docx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#021     Updating Gantt Chart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#022     Downloading git_log.txt </t>
   </si>
 </sst>
 </file>
@@ -639,6 +639,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -650,33 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1080,26 +1080,26 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BT9" activeCellId="1" sqref="DD12 BT9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
-    <col min="42" max="42" width="2.75" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="42" max="42" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1107,55 +1107,55 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="K2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="33"/>
+      <c r="Q2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="29"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="37"/>
+      <c r="V2" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AA2" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AJ2" s="23"/>
       <c r="AK2" s="23"/>
@@ -1165,24 +1165,24 @@
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>19</v>
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>12</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1207,13 +1207,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1395,9 +1395,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1415,9 +1415,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:67" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
@@ -1435,9 +1435,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:67" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -1455,9 +1455,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:67" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
@@ -1475,9 +1475,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:67" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7">
         <v>9</v>
@@ -1495,9 +1495,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:67" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C10" s="7">
         <v>10</v>
@@ -1515,9 +1515,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:67" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C11" s="7">
         <v>12</v>
@@ -1535,9 +1535,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:67" ht="73.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7">
         <v>14</v>
@@ -1555,9 +1555,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:67" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C13" s="7">
         <v>16</v>
@@ -1575,9 +1575,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:67" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C14" s="7">
         <v>18</v>
@@ -1595,9 +1595,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:67" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C15" s="9">
         <v>21</v>
@@ -1615,9 +1615,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:67" ht="60.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C16" s="7">
         <v>21</v>
@@ -1635,157 +1635,229 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7">
         <v>22</v>
       </c>
       <c r="D17" s="7">
-        <v>26</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="E17" s="7">
+        <v>24</v>
+      </c>
+      <c r="F17" s="7">
+        <v>25</v>
+      </c>
       <c r="G17" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7">
+        <v>25</v>
+      </c>
+      <c r="F18" s="7">
+        <v>27</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="7">
+        <v>27</v>
+      </c>
+      <c r="D19" s="7">
+        <v>29</v>
+      </c>
+      <c r="E19" s="7">
+        <v>27</v>
+      </c>
+      <c r="F19" s="7">
+        <v>28</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="7">
+        <v>29</v>
+      </c>
+      <c r="D20" s="7">
+        <v>31</v>
+      </c>
+      <c r="E20" s="7">
+        <v>28</v>
+      </c>
+      <c r="F20" s="7">
+        <v>30</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="7">
+        <v>31</v>
+      </c>
+      <c r="D21" s="7">
+        <v>33</v>
+      </c>
+      <c r="E21" s="7">
+        <v>30</v>
+      </c>
+      <c r="F21" s="7">
+        <v>32</v>
+      </c>
+      <c r="G21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="7">
+        <v>33</v>
+      </c>
+      <c r="D22" s="7">
+        <v>36</v>
+      </c>
+      <c r="E22" s="7">
+        <v>32</v>
+      </c>
+      <c r="F22" s="7">
+        <v>36</v>
+      </c>
+      <c r="G22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="7">
-        <v>26</v>
-      </c>
-      <c r="D18" s="7">
-        <v>28</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="C23" s="7">
+        <v>36</v>
+      </c>
+      <c r="D23" s="7">
+        <v>38</v>
+      </c>
+      <c r="E23" s="7">
+        <v>36</v>
+      </c>
+      <c r="F23" s="7">
+        <v>38</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="7">
-        <v>28</v>
-      </c>
-      <c r="D19" s="7">
-        <v>31</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+      <c r="C24" s="7">
+        <v>38</v>
+      </c>
+      <c r="D24" s="7">
+        <v>39</v>
+      </c>
+      <c r="E24" s="7">
+        <v>38</v>
+      </c>
+      <c r="F24" s="7">
+        <v>40</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="7">
+        <v>39</v>
+      </c>
+      <c r="D25" s="7">
+        <v>40</v>
+      </c>
+      <c r="E25" s="7">
+        <v>40</v>
+      </c>
+      <c r="F25" s="7">
+        <v>41</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="7">
+        <v>40</v>
+      </c>
+      <c r="D26" s="7">
+        <v>41</v>
+      </c>
+      <c r="E26" s="7">
+        <v>41</v>
+      </c>
+      <c r="F26" s="7">
+        <v>41</v>
+      </c>
+      <c r="G26" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="7">
-        <v>31</v>
-      </c>
-      <c r="D20" s="7">
-        <v>33</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
+      <c r="C27" s="7">
+        <v>41</v>
+      </c>
+      <c r="D27" s="7">
+        <v>41</v>
+      </c>
+      <c r="E27" s="7">
+        <v>41</v>
+      </c>
+      <c r="F27" s="7">
+        <v>41</v>
+      </c>
+      <c r="G27" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1795,9 +1867,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1807,9 +1879,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1819,9 +1891,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1831,9 +1903,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1843,9 +1915,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1855,9 +1927,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1867,9 +1939,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1879,9 +1951,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1891,9 +1963,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1903,9 +1975,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1915,9 +1987,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1929,17 +2001,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>